<commit_message>
added Departure and Arrival
</commit_message>
<xml_diff>
--- a/select_gares.xlsx
+++ b/select_gares.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathanodic/Dev/Python/SNCFCollection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08D848C-030E-514C-9D7F-CE8DB853BB71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5324E8F-0B4E-044E-9026-61BA3E47FC61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -542,7 +542,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>